<commit_message>
Fix: Backward compatibility for old Excel column names
- Added automatic column renaming for old format files
- Supports both 'Data Nașterii' and 'Data nașterii' formats
- Automatically converts old files to new format on load
- Regenerated dummy data with correct column names
- Fixes 'Structura fișierului este invalidă' error
</commit_message>
<xml_diff>
--- a/date_dummy_30_certificate.xlsx
+++ b/date_dummy_30_certificate.xlsx
@@ -463,32 +463,32 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Data Nașterii</t>
+          <t>Data nașterii</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Serie Certificat</t>
+          <t>Serie certificat</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Număr Certificat</t>
+          <t>Număr certificat</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Nivel Certificat</t>
+          <t>Nivel certificat</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Data Eliberare</t>
+          <t>Data eliberare</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Data Expirare</t>
+          <t>Data expirare</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -500,7 +500,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>General de Armată</t>
+          <t>General de Brigadă</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -515,44 +515,40 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>29.01.1972</t>
+          <t>06.05.1989</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>416714</t>
+          <t>320794</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SSv</t>
+          <t>S</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>16.01.2024</t>
+          <t>09.08.2022</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>26.01.2026</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Documentație completă</t>
-        </is>
-      </c>
+          <t>26.07.2026</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Major</t>
+          <t>Plutonier Major</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -567,17 +563,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>05.11.1991</t>
+          <t>25.04.1988</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>IJ</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>555939</t>
+          <t>940928</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -587,20 +583,24 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>14.09.2022</t>
+          <t>26.02.2021</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>17.02.2026</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
+          <t>04.02.2026</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Contact: 0721234567</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>General de Divizie</t>
+          <t>Soldat</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -615,17 +615,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14.07.1985</t>
+          <t>24.07.2000</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>QR</t>
+          <t>GH</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>956481</t>
+          <t>732516</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -635,12 +635,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>17.11.2022</t>
+          <t>04.01.2021</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>05.07.2025</t>
+          <t>29.11.2025</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -648,7 +648,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>General de Divizie</t>
+          <t>Colonel</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -663,17 +663,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12.02.2000</t>
+          <t>22.07.1987</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>GH</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>945965</t>
+          <t>968263</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -683,12 +683,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>09.07.2023</t>
+          <t>07.01.2021</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>27.12.2025</t>
+          <t>13.11.2027</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -696,7 +696,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sergent Major</t>
+          <t>General de Armată</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -711,44 +711,44 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14.04.1995</t>
+          <t>15.11.1989</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>KL</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>753963</t>
+          <t>910921</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>SSID</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>13.02.2023</t>
+          <t>24.10.2022</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>23.04.2026</t>
+          <t>22.11.2027</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Contact: 0721234567</t>
+          <t>Documentație completă</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Plutonier Major</t>
+          <t>Plutonier Adjutant</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -763,44 +763,40 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>11.01.1987</t>
+          <t>08.02.1984</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>GH</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>190248</t>
+          <t>811444</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>SSID</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>07.11.2024</t>
+          <t>12.09.2022</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>26.09.2025</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Verificat</t>
-        </is>
-      </c>
+          <t>25.02.2026</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Caporal</t>
+          <t>Soldat</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -815,17 +811,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>24.01.1975</t>
+          <t>04.09.1992</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>EF</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>738756</t>
+          <t>501952</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -835,24 +831,24 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>28.03.2021</t>
+          <t>21.03.2021</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>04.01.2026</t>
+          <t>14.04.2026</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Documentație completă</t>
+          <t>Verificat</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>General de Divizie</t>
+          <t>Caporal</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -867,44 +863,44 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>16.10.1973</t>
+          <t>27.07.1974</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>485219</t>
+          <t>710600</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>SSv</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>25.04.2021</t>
+          <t>05.10.2024</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>08.12.2025</t>
+          <t>16.05.2026</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Verificat</t>
+          <t>Contact: 0721234567</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Caporal</t>
+          <t>Plutonier Adjutant Principal</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -919,40 +915,44 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>05.06.1970</t>
+          <t>03.01.1972</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>KL</t>
+          <t>CD</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>976212</t>
+          <t>594858</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>S</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>07.05.2024</t>
+          <t>16.06.2022</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>18.12.2026</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr"/>
+          <t>07.07.2025</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nivel actualizat</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sergent Major</t>
+          <t>Locotenent</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -967,40 +967,44 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>10.10.2000</t>
+          <t>22.07.1989</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>QR</t>
+          <t>EF</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>580334</t>
+          <t>541294</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>SSv</t>
+          <t>SSID</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>02.12.2020</t>
+          <t>01.06.2023</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>27.09.2025</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr"/>
+          <t>13.10.2027</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Contact: 0721234567</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Sublocotenent</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1015,7 +1019,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>25.01.1974</t>
+          <t>01.03.1974</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1025,7 +1029,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>363418</t>
+          <t>184656</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1035,24 +1039,24 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>19.11.2023</t>
+          <t>23.05.2023</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>29.05.2026</t>
+          <t>29.01.2026</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Verificat</t>
+          <t>Reînnoire în curs</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>General de Divizie</t>
+          <t>Sergent Major</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1067,44 +1071,40 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>26.12.1971</t>
+          <t>22.07.1981</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>IJ</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>297994</t>
+          <t>884872</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>SS</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>19.08.2021</t>
+          <t>06.01.2023</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>01.12.2025</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Verificat</t>
-        </is>
-      </c>
+          <t>31.08.2026</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Plutonier Major</t>
+          <t>General de Divizie</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1119,44 +1119,44 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>28.08.1976</t>
+          <t>09.08.1990</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>KL</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>705200</t>
+          <t>430909</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>SSID</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>12.09.2022</t>
+          <t>09.12.2021</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>12.01.2026</t>
+          <t>18.01.2026</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Nivel actualizat</t>
+          <t>Documentație completă</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Plutonier Adjutant Principal</t>
+          <t>Sergent Major</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>05.11.1973</t>
+          <t>01.11.1977</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1181,30 +1181,34 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>141161</t>
+          <t>366944</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>SSID</t>
+          <t>S</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>08.11.2021</t>
+          <t>14.07.2021</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>09.08.2027</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr"/>
+          <t>19.11.2027</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Documentație completă</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Locotenent</t>
+          <t>General de Armată</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1219,17 +1223,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>06.07.1978</t>
+          <t>12.04.1996</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>IJ</t>
+          <t>EF</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>492234</t>
+          <t>703599</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1239,24 +1243,20 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>12.02.2023</t>
+          <t>19.03.2023</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>21.02.2027</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Documentație completă</t>
-        </is>
-      </c>
+          <t>04.12.2025</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Căpitan</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1271,17 +1271,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>02.05.1973</t>
+          <t>20.02.1989</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>QR</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>759465</t>
+          <t>414673</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1291,20 +1291,24 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>01.03.2022</t>
+          <t>06.11.2022</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>12.01.2026</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr"/>
+          <t>02.02.2026</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Documentație completă</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Sergent Major</t>
+          <t>Căpitan</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1319,44 +1323,44 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>06.07.1983</t>
+          <t>13.02.1977</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>CD</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>909563</t>
+          <t>383538</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>SSID</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>28.02.2022</t>
+          <t>16.12.2020</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>17.12.2026</t>
+          <t>14.04.2026</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Nivel actualizat</t>
+          <t>Documentație completă</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Sublocotenent</t>
+          <t>General de Brigadă</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1371,17 +1375,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>16.01.1990</t>
+          <t>10.06.1985</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>IJ</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>567345</t>
+          <t>332754</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1391,20 +1395,24 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>23.12.2020</t>
+          <t>14.05.2023</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>09.06.2026</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr"/>
+          <t>23.02.2026</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Reînnoire în curs</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sergent Major</t>
+          <t>Sergent</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1419,44 +1427,44 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12.03.1979</t>
+          <t>03.02.1970</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>EF</t>
+          <t>KL</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>500889</t>
+          <t>925109</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>SSv</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>14.02.2021</t>
+          <t>06.12.2023</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>08.07.2027</t>
+          <t>28.12.2025</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Nivel actualizat</t>
+          <t>Documentație completă</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Plutonier Adjutant</t>
+          <t>Plutonier Adjutant Principal</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1471,44 +1479,40 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>19.12.1989</t>
+          <t>15.04.1987</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>IJ</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>229933</t>
+          <t>750142</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>SSID</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>18.10.2021</t>
+          <t>23.07.2022</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>13.02.2026</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Verificat</t>
-        </is>
-      </c>
+          <t>18.09.2025</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Plutonier Major</t>
+          <t>Sergent Major</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1523,44 +1527,44 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>30.06.1985</t>
+          <t>01.07.1988</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>763528</t>
+          <t>750155</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>SSv</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>25.05.2024</t>
+          <t>13.10.2021</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>20.07.2025</t>
+          <t>21.02.2027</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Verificat</t>
+          <t>Reînnoire în curs</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Soldat</t>
+          <t>Plutonier Adjutant</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1575,40 +1579,44 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>28.11.1994</t>
+          <t>17.05.1985</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>KL</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>902209</t>
+          <t>171799</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>S</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>25.04.2021</t>
+          <t>28.04.2021</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>31.01.2026</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr"/>
+          <t>08.01.2026</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Reînnoire în curs</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Locotenent</t>
+          <t>Locotenent Colonel</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1623,40 +1631,44 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>10.09.1984</t>
+          <t>28.03.1986</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>QR</t>
+          <t>IJ</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>774656</t>
+          <t>257178</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>SSv</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>22.12.2021</t>
+          <t>20.03.2024</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>17.12.2025</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr"/>
+          <t>27.04.2026</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Nivel actualizat</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Sergent Major</t>
+          <t>Plutonier Major</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1671,44 +1683,40 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>26.04.1974</t>
+          <t>21.01.1988</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>IJ</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>256875</t>
+          <t>716701</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>SSv</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>17.06.2023</t>
+          <t>17.01.2023</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>06.12.2025</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>Documentație completă</t>
-        </is>
-      </c>
+          <t>09.12.2025</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Locotenent Colonel</t>
+          <t>Colonel</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1723,32 +1731,32 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>22.01.1989</t>
+          <t>05.10.2000</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>289415</t>
+          <t>925162</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>SSID</t>
+          <t>SSv</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>17.05.2021</t>
+          <t>10.07.2022</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>29.11.2026</t>
+          <t>19.07.2027</t>
         </is>
       </c>
       <c r="J26" t="inlineStr"/>
@@ -1756,7 +1764,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Sergent Major</t>
+          <t>General</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1771,40 +1779,44 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>13.06.1984</t>
+          <t>11.09.1980</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>GH</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>167788</t>
+          <t>608573</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>S</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>04.07.2021</t>
+          <t>20.10.2024</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>23.07.2026</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr"/>
+          <t>14.09.2025</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Contact: 0721234567</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Sublocotenent</t>
+          <t>Colonel</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1819,44 +1831,44 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>07.04.1975</t>
+          <t>21.07.1986</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>CD</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>547757</t>
+          <t>353762</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>SS</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>29.10.2021</t>
+          <t>11.11.2022</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>20.02.2026</t>
+          <t>16.12.2025</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Reînnoire în curs</t>
+          <t>Nivel actualizat</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Plutonier Adjutant</t>
+          <t>Plutonier Major</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1871,17 +1883,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>24.08.1995</t>
+          <t>14.08.1995</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>KL</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>321496</t>
+          <t>611655</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1891,12 +1903,12 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>11.11.2023</t>
+          <t>15.04.2023</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>21.03.2027</t>
+          <t>21.12.2025</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -1908,7 +1920,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Căpitan</t>
+          <t>Plutonier Major</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1923,17 +1935,17 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14.08.1988</t>
+          <t>25.12.1998</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>158299</t>
+          <t>630063</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1943,17 +1955,17 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>06.12.2021</t>
+          <t>23.07.2023</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>25.11.2027</t>
+          <t>23.01.2026</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Verificat</t>
+          <t>Reînnoire în curs</t>
         </is>
       </c>
     </row>
@@ -1975,37 +1987,37 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>18.03.1997</t>
+          <t>17.05.1978</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>410320</t>
+          <t>128332</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>S</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>30.03.2024</t>
+          <t>05.06.2022</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>08.12.2025</t>
+          <t>13.11.2025</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Reînnoire în curs</t>
+          <t>Documentație completă</t>
         </is>
       </c>
     </row>

</xml_diff>